<commit_message>
Testing the output of generated xml
</commit_message>
<xml_diff>
--- a/spec/fixtures/example_manifest_loads/object_one/metadata.xlsx
+++ b/spec/fixtures/example_manifest_loads/object_one/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgalarza/code/bulwark/spec/fixtures/example_manifest_loads/object_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB346FC-5270-5F4E-B92B-A6AB3D20DDB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1F1443-B27A-5E47-94BA-871AE0FA2AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2760" windowWidth="27640" windowHeight="16940" xr2:uid="{544C3912-5CC3-F541-A5DE-1377C76C530B}"/>
+    <workbookView xWindow="13280" yWindow="1760" windowWidth="27640" windowHeight="16940" xr2:uid="{544C3912-5CC3-F541-A5DE-1377C76C530B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Coll / Box #</t>
   </si>
@@ -88,25 +88,52 @@
   </si>
   <si>
     <t>front.tif; back.tif</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>J. Rosenblatt &amp; Co.</t>
+  </si>
+  <si>
+    <t>Trade cards</t>
+  </si>
+  <si>
+    <t>Arc.MS.56</t>
+  </si>
+  <si>
+    <t>Arnold and Deanne Kaplan Collection of Early American Judaica (University of Pennsylvania)</t>
+  </si>
+  <si>
+    <t>undated</t>
+  </si>
+  <si>
+    <t>Baltimore, Maryland, United States | Maryland, United States</t>
+  </si>
+  <si>
+    <t>http://rightsstatements.org/page/NoC-US/1.0/?</t>
+  </si>
+  <si>
+    <t>J. Rosenblatt &amp; Co.: Importers: Earthenware, China, Majolica, Novelties | 32 South Howard Street, Baltimore, MD</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>House furnishings | Jewish merchants | Trade cards (advertising)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,7 +158,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,86 +473,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92148881-0C0D-484B-A289-7EE43A37FD2F}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="82.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>